<commit_message>
Enhance heuristic solution with detailed cost calculations and in-transit inventory handling. Added debug prints for data dimensions and costs, and updated Excel output to include purchasing costs and shipping details.
</commit_message>
<xml_diff>
--- a/heuristic_results.xlsx
+++ b/heuristic_results.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orders" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventory" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Containers" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Purchasing Costs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orders" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventory" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Containers" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,26 +456,56 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19074970</v>
+        <v>15252220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Number of Products</t>
+          <t>Total Purchasing Cost</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>15232000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Total Air Shipping Cost</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Total Ocean Shipping Cost</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Number of Products</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Number of Periods</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B7" t="n">
         <v>6</v>
       </c>
     </row>
@@ -489,7 +520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,460 +536,158 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Order Period</t>
+          <t>Unit Cost</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Shipping Method</t>
+          <t>Total Quantity</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Order Quantity</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Total Volume</t>
+          <t>Total Purchasing Cost</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>5000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>38</v>
       </c>
       <c r="D2" t="n">
-        <v>104</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6.552</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>2000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>45</v>
       </c>
       <c r="D3" t="n">
-        <v>61</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5.002</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>9000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>282</v>
       </c>
       <c r="D4" t="n">
-        <v>200</v>
-      </c>
-      <c r="E4" t="n">
-        <v>19.6</v>
+        <v>2538000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Air</t>
-        </is>
+        <v>9000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>252</v>
       </c>
       <c r="D5" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.352</v>
+        <v>2268000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>2000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>116</v>
       </c>
       <c r="D6" t="n">
-        <v>102</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4.385999999999999</v>
+        <v>232000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>9000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>154</v>
       </c>
       <c r="D7" t="n">
-        <v>146</v>
-      </c>
-      <c r="E7" t="n">
-        <v>9.198</v>
+        <v>1386000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>7000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>172</v>
       </c>
       <c r="D8" t="n">
-        <v>67</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3.015</v>
+        <v>1204000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>5000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>261</v>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.032</v>
+        <v>1305000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>9000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>94</v>
       </c>
       <c r="D10" t="n">
-        <v>70</v>
-      </c>
-      <c r="E10" t="n">
-        <v>5.53</v>
+        <v>846000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
+        <v>7000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>739</v>
       </c>
       <c r="D11" t="n">
-        <v>168</v>
-      </c>
-      <c r="E11" t="n">
-        <v>13.776</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>9</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>65</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4.42</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>10</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>154</v>
-      </c>
-      <c r="E13" t="n">
-        <v>15.092</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Air</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>162</v>
-      </c>
-      <c r="E14" t="n">
-        <v>15.876</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>38</v>
-      </c>
-      <c r="E15" t="n">
-        <v>2.774</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" t="n">
-        <v>3</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>93</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.465</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>3</v>
-      </c>
-      <c r="B17" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>200</v>
-      </c>
-      <c r="E17" t="n">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>4</v>
-      </c>
-      <c r="B18" t="n">
-        <v>3</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>155</v>
-      </c>
-      <c r="E18" t="n">
-        <v>9.765000000000001</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>5</v>
-      </c>
-      <c r="B19" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>49</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2.205</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>6</v>
-      </c>
-      <c r="B20" t="n">
-        <v>3</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>183</v>
-      </c>
-      <c r="E20" t="n">
-        <v>15.738</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>7</v>
-      </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>175</v>
-      </c>
-      <c r="E21" t="n">
-        <v>13.825</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>8</v>
-      </c>
-      <c r="B22" t="n">
-        <v>3</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>32</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2.624</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>9</v>
-      </c>
-      <c r="B23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>172</v>
-      </c>
-      <c r="E23" t="n">
-        <v>11.696</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>10</v>
-      </c>
-      <c r="B24" t="n">
-        <v>3</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Ocean</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>199</v>
-      </c>
-      <c r="E24" t="n">
-        <v>19.502</v>
+        <v>5173000</v>
       </c>
     </row>
   </sheetData>
@@ -967,6 +696,599 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Order Period</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Shipping Method</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Order Quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total Volume</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Purchasing Cost</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Shipping Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>61</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.002</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>305000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1400000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.352</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>168000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>82</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.526</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>738000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>97</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6.111</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>873000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>67</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.015</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>134000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>168</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.776</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>840000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>154</v>
+      </c>
+      <c r="E9" t="n">
+        <v>15.092</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1078000</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>162</v>
+      </c>
+      <c r="E10" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="F10" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1134000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>38</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.774</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>190000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>45</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>90000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>200</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>155</v>
+      </c>
+      <c r="E14" t="n">
+        <v>9.765000000000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1395000</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>49</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.205</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>98000</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>154</v>
+      </c>
+      <c r="E16" t="n">
+        <v>13.244</v>
+      </c>
+      <c r="F16" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1386000</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>172</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.588</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1204000</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>32</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.624</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>160000</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>94</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6.392</v>
+      </c>
+      <c r="F19" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>846000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>199</v>
+      </c>
+      <c r="E20" t="n">
+        <v>19.502</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1393000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1236,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="n">
-        <v>241</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24">
@@ -1258,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>27</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26">
@@ -1280,7 +1602,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>231</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28">
@@ -1291,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29">
@@ -1313,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>192</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31">
@@ -1346,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34">
@@ -1357,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35">
@@ -1368,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36">
@@ -1390,7 +1712,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>104</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38">
@@ -1401,7 +1723,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>49</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39">
@@ -1423,7 +1745,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>16</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41">
@@ -1456,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44">
@@ -1500,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48">
@@ -1511,7 +1833,7 @@
         <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -1533,7 +1855,7 @@
         <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51">
@@ -1662,7 +1984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1698,10 +2020,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>5500</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Enhance heuristic_solution.py by adding express shipping cost calculations and improving inventory management. Updated total cost calculations to include holding and fixed costs, and modified Excel output to reflect detailed cost breakdowns and quantities. Improved debug output for better traceability of costs and inventory changes.
</commit_message>
<xml_diff>
--- a/heuristic_results.xlsx
+++ b/heuristic_results.xlsx
@@ -8,10 +8,11 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Purchasing Costs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orders" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventory" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Containers" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Quantities Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Purchasing Costs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orders" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventory" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Containers" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15252220</v>
+        <v>16515758</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +477,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3720</v>
+        <v>8418</v>
       </c>
     </row>
     <row r="5">
@@ -492,21 +493,71 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Number of Products</t>
+          <t>Total Holding Cost</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>1256400</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Total Fixed Cost</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Number of Products</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Number of Periods</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B9" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Total Quantity Ordered (All Products)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total Ocean Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Total Air Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,17 +587,42 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Total Quantity</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ocean Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Air Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Unit Cost</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Quantity</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Total Purchasing Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total Volume</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ocean Volume</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Air Volume</t>
         </is>
       </c>
     </row>
@@ -555,13 +631,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5000</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
         <v>38</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F2" t="n">
         <v>190000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.774</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.774</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -569,13 +660,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2000</v>
+        <v>45</v>
       </c>
       <c r="C3" t="n">
         <v>45</v>
       </c>
       <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F3" t="n">
         <v>90000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -583,13 +689,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>9000</v>
+        <v>282</v>
       </c>
       <c r="C4" t="n">
         <v>282</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F4" t="n">
         <v>2538000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12.126</v>
+      </c>
+      <c r="H4" t="n">
+        <v>12.126</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -597,13 +718,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>9000</v>
+        <v>252</v>
       </c>
       <c r="C5" t="n">
         <v>252</v>
       </c>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F5" t="n">
         <v>2268000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="H5" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -611,13 +747,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2000</v>
+        <v>116</v>
       </c>
       <c r="C6" t="n">
         <v>116</v>
       </c>
       <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F6" t="n">
         <v>232000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -625,13 +776,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>9000</v>
+        <v>154</v>
       </c>
       <c r="C7" t="n">
         <v>154</v>
       </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F7" t="n">
         <v>1386000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>13.244</v>
+      </c>
+      <c r="H7" t="n">
+        <v>13.244</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -639,13 +805,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7000</v>
+        <v>172</v>
       </c>
       <c r="C8" t="n">
         <v>172</v>
       </c>
       <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="F8" t="n">
         <v>1204000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>13.588</v>
+      </c>
+      <c r="H8" t="n">
+        <v>13.588</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -653,13 +834,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5000</v>
+        <v>261</v>
       </c>
       <c r="C9" t="n">
         <v>261</v>
       </c>
       <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F9" t="n">
         <v>1305000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>21.402</v>
+      </c>
+      <c r="H9" t="n">
+        <v>21.402</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -667,13 +863,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>9000</v>
+        <v>94</v>
       </c>
       <c r="C10" t="n">
         <v>94</v>
       </c>
       <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F10" t="n">
         <v>846000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6.392</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6.392</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -681,13 +892,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
+        <v>739</v>
+      </c>
+      <c r="C11" t="n">
+        <v>553</v>
+      </c>
+      <c r="D11" t="n">
+        <v>186</v>
+      </c>
+      <c r="E11" t="n">
         <v>7000</v>
       </c>
-      <c r="C11" t="n">
-        <v>739</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="F11" t="n">
         <v>5173000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>72.422</v>
+      </c>
+      <c r="H11" t="n">
+        <v>54.194</v>
+      </c>
+      <c r="I11" t="n">
+        <v>18.228</v>
       </c>
     </row>
   </sheetData>
@@ -696,6 +922,327 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Cost</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ocean Quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Air Quantity</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total Purchasing Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total Holding Cost</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total Fixed Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>38</v>
+      </c>
+      <c r="D2" t="n">
+        <v>38</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>190000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H2" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>45</v>
+      </c>
+      <c r="D3" t="n">
+        <v>45</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>90000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H3" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>282</v>
+      </c>
+      <c r="D4" t="n">
+        <v>282</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2538000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H4" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>252</v>
+      </c>
+      <c r="D5" t="n">
+        <v>252</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2268000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H5" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>116</v>
+      </c>
+      <c r="D6" t="n">
+        <v>116</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>232000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H6" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>154</v>
+      </c>
+      <c r="D7" t="n">
+        <v>154</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1386000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H7" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>172</v>
+      </c>
+      <c r="D8" t="n">
+        <v>172</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1204000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H8" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>261</v>
+      </c>
+      <c r="D9" t="n">
+        <v>261</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1305000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H9" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>94</v>
+      </c>
+      <c r="D10" t="n">
+        <v>94</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>846000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H10" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>7000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>739</v>
+      </c>
+      <c r="D11" t="n">
+        <v>553</v>
+      </c>
+      <c r="E11" t="n">
+        <v>186</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5173000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>125640</v>
+      </c>
+      <c r="H11" t="n">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1288,7 +1835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1448,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>309</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14">
@@ -1470,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>105</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16">
@@ -1492,7 +2039,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>338</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18">
@@ -1503,7 +2050,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>184</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19">
@@ -1525,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>380</v>
+        <v>489</v>
       </c>
     </row>
     <row r="21">
@@ -1569,7 +2116,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25">
@@ -1602,7 +2149,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>249</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28">
@@ -1613,7 +2160,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>193</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29">
@@ -1635,7 +2182,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>301</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31">
@@ -1984,7 +2531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Update heuristic_solution.py to support express shipping with corresponding cost calculations and inventory management. Adjusted total cost calculations to include express shipping and updated Excel output to reflect new shipping methods and detailed cost breakdowns. Enhanced debug output for clarity on inventory and shipping costs.
</commit_message>
<xml_diff>
--- a/heuristic_results.xlsx
+++ b/heuristic_results.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16515758</v>
+        <v>16617176</v>
       </c>
     </row>
     <row r="3">
@@ -477,87 +477,107 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8418</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Total Ocean Shipping Cost</t>
+          <t>Total Express Shipping Cost</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16500</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Total Holding Cost</t>
+          <t>Total Ocean Shipping Cost</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1256400</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Total Fixed Cost</t>
+          <t>Total Holding Cost</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2440</v>
+        <v>1361680</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Number of Products</t>
+          <t>Total Fixed Cost</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Number of Periods</t>
+          <t>Number of Products</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total Quantity Ordered (All Products)</t>
+          <t>Number of Periods</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2153</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Total Ocean Shipping Quantity</t>
+          <t>Total Quantity Ordered (All Products)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1967</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Total Ocean Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Total Air Shipping Quantity</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>186</v>
+      <c r="B13" t="n">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Total Express Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -566,6 +586,432 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Quantity</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ocean Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Air Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Express Shipping Quantity</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total Purchasing Cost</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total Volume</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Ocean Volume</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Air Volume</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Express Volume</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>38</v>
+      </c>
+      <c r="C2" t="n">
+        <v>38</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>190000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.774</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.774</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>45</v>
+      </c>
+      <c r="C3" t="n">
+        <v>45</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>90000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>282</v>
+      </c>
+      <c r="C4" t="n">
+        <v>282</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2538000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>12.126</v>
+      </c>
+      <c r="I4" t="n">
+        <v>12.126</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>252</v>
+      </c>
+      <c r="C5" t="n">
+        <v>252</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2268000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="I5" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>116</v>
+      </c>
+      <c r="C6" t="n">
+        <v>116</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>232000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>154</v>
+      </c>
+      <c r="C7" t="n">
+        <v>154</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1386000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>13.244</v>
+      </c>
+      <c r="I7" t="n">
+        <v>13.244</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>172</v>
+      </c>
+      <c r="C8" t="n">
+        <v>172</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1204000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>13.588</v>
+      </c>
+      <c r="I8" t="n">
+        <v>13.588</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>261</v>
+      </c>
+      <c r="C9" t="n">
+        <v>261</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1305000</v>
+      </c>
+      <c r="H9" t="n">
+        <v>21.402</v>
+      </c>
+      <c r="I9" t="n">
+        <v>21.402</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>94</v>
+      </c>
+      <c r="C10" t="n">
+        <v>94</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>846000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6.392</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6.392</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>739</v>
+      </c>
+      <c r="C11" t="n">
+        <v>553</v>
+      </c>
+      <c r="D11" t="n">
+        <v>162</v>
+      </c>
+      <c r="E11" t="n">
+        <v>24</v>
+      </c>
+      <c r="F11" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5173000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>72.422</v>
+      </c>
+      <c r="I11" t="n">
+        <v>54.194</v>
+      </c>
+      <c r="J11" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -587,42 +1033,42 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unit Cost</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Total Quantity</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Ocean Shipping Quantity</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Air Shipping Quantity</t>
+          <t>Ocean Quantity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Unit Cost</t>
+          <t>Air Quantity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Express Quantity</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Total Purchasing Cost</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Total Volume</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Ocean Volume</t>
+          <t>Total Holding Cost</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Air Volume</t>
+          <t>Total Fixed Cost</t>
         </is>
       </c>
     </row>
@@ -631,28 +1077,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>5000</v>
       </c>
       <c r="C2" t="n">
         <v>38</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E2" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>190000</v>
       </c>
-      <c r="G2" t="n">
-        <v>2.774</v>
-      </c>
       <c r="H2" t="n">
-        <v>2.774</v>
+        <v>136168</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
@@ -660,28 +1106,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>45</v>
+        <v>2000</v>
       </c>
       <c r="C3" t="n">
         <v>45</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E3" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
         <v>90000</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.225</v>
-      </c>
       <c r="H3" t="n">
-        <v>0.225</v>
+        <v>136168</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4">
@@ -689,28 +1135,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>282</v>
+        <v>9000</v>
       </c>
       <c r="C4" t="n">
         <v>282</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>282</v>
       </c>
       <c r="E4" t="n">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>2538000</v>
       </c>
-      <c r="G4" t="n">
-        <v>12.126</v>
-      </c>
       <c r="H4" t="n">
-        <v>12.126</v>
+        <v>136168</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5">
@@ -718,28 +1164,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>252</v>
+        <v>9000</v>
       </c>
       <c r="C5" t="n">
         <v>252</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="E5" t="n">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>2268000</v>
       </c>
-      <c r="G5" t="n">
-        <v>15.876</v>
-      </c>
       <c r="H5" t="n">
-        <v>15.876</v>
+        <v>136168</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6">
@@ -747,28 +1193,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>116</v>
+        <v>2000</v>
       </c>
       <c r="C6" t="n">
         <v>116</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="E6" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
         <v>232000</v>
       </c>
-      <c r="G6" t="n">
-        <v>5.22</v>
-      </c>
       <c r="H6" t="n">
-        <v>5.22</v>
+        <v>136168</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7">
@@ -776,28 +1222,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>154</v>
+        <v>9000</v>
       </c>
       <c r="C7" t="n">
         <v>154</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="E7" t="n">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
         <v>1386000</v>
       </c>
-      <c r="G7" t="n">
-        <v>13.244</v>
-      </c>
       <c r="H7" t="n">
-        <v>13.244</v>
+        <v>136168</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8">
@@ -805,28 +1251,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>172</v>
+        <v>7000</v>
       </c>
       <c r="C8" t="n">
         <v>172</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E8" t="n">
-        <v>7000</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
         <v>1204000</v>
       </c>
-      <c r="G8" t="n">
-        <v>13.588</v>
-      </c>
       <c r="H8" t="n">
-        <v>13.588</v>
+        <v>136168</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9">
@@ -834,28 +1280,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>261</v>
+        <v>5000</v>
       </c>
       <c r="C9" t="n">
         <v>261</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>261</v>
       </c>
       <c r="E9" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
         <v>1305000</v>
       </c>
-      <c r="G9" t="n">
-        <v>21.402</v>
-      </c>
       <c r="H9" t="n">
-        <v>21.402</v>
+        <v>136168</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10">
@@ -863,28 +1309,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>94</v>
+        <v>9000</v>
       </c>
       <c r="C10" t="n">
         <v>94</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="E10" t="n">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
         <v>846000</v>
       </c>
-      <c r="G10" t="n">
-        <v>6.392</v>
-      </c>
       <c r="H10" t="n">
-        <v>6.392</v>
+        <v>136168</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11">
@@ -892,330 +1338,6 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>739</v>
-      </c>
-      <c r="C11" t="n">
-        <v>553</v>
-      </c>
-      <c r="D11" t="n">
-        <v>186</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7000</v>
-      </c>
-      <c r="F11" t="n">
-        <v>5173000</v>
-      </c>
-      <c r="G11" t="n">
-        <v>72.422</v>
-      </c>
-      <c r="H11" t="n">
-        <v>54.194</v>
-      </c>
-      <c r="I11" t="n">
-        <v>18.228</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Unit Cost</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Quantity</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ocean Quantity</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Air Quantity</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total Purchasing Cost</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Total Holding Cost</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Total Fixed Cost</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>38</v>
-      </c>
-      <c r="D2" t="n">
-        <v>38</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>190000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H2" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>45</v>
-      </c>
-      <c r="D3" t="n">
-        <v>45</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>90000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H3" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>282</v>
-      </c>
-      <c r="D4" t="n">
-        <v>282</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2538000</v>
-      </c>
-      <c r="G4" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H4" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C5" t="n">
-        <v>252</v>
-      </c>
-      <c r="D5" t="n">
-        <v>252</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2268000</v>
-      </c>
-      <c r="G5" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H5" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C6" t="n">
-        <v>116</v>
-      </c>
-      <c r="D6" t="n">
-        <v>116</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>232000</v>
-      </c>
-      <c r="G6" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H6" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C7" t="n">
-        <v>154</v>
-      </c>
-      <c r="D7" t="n">
-        <v>154</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1386000</v>
-      </c>
-      <c r="G7" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H7" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7000</v>
-      </c>
-      <c r="C8" t="n">
-        <v>172</v>
-      </c>
-      <c r="D8" t="n">
-        <v>172</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1204000</v>
-      </c>
-      <c r="G8" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H8" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C9" t="n">
-        <v>261</v>
-      </c>
-      <c r="D9" t="n">
-        <v>261</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1305000</v>
-      </c>
-      <c r="G9" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H9" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9000</v>
-      </c>
-      <c r="C10" t="n">
-        <v>94</v>
-      </c>
-      <c r="D10" t="n">
-        <v>94</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>846000</v>
-      </c>
-      <c r="G10" t="n">
-        <v>125640</v>
-      </c>
-      <c r="H10" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
         <v>7000</v>
       </c>
       <c r="C11" t="n">
@@ -1225,16 +1347,19 @@
         <v>553</v>
       </c>
       <c r="E11" t="n">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="F11" t="n">
+        <v>24</v>
+      </c>
+      <c r="G11" t="n">
         <v>5173000</v>
       </c>
-      <c r="G11" t="n">
-        <v>125640</v>
-      </c>
       <c r="H11" t="n">
-        <v>244</v>
+        <v>136168</v>
+      </c>
+      <c r="I11" t="n">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +1373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1311,16 +1436,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E2" t="n">
-        <v>5.002</v>
+        <v>5.248</v>
       </c>
       <c r="F2" t="n">
         <v>5000</v>
       </c>
       <c r="G2" t="n">
-        <v>305000</v>
+        <v>320000</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1363,7 +1488,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Air</t>
+          <t>Express</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1379,7 +1504,7 @@
         <v>168000</v>
       </c>
       <c r="H4" t="n">
-        <v>480</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1395,16 +1520,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>82</v>
+        <v>212</v>
       </c>
       <c r="E5" t="n">
-        <v>3.526</v>
+        <v>9.116</v>
       </c>
       <c r="F5" t="n">
         <v>9000</v>
       </c>
       <c r="G5" t="n">
-        <v>738000</v>
+        <v>1908000</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -1468,7 +1593,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1479,16 +1604,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>168</v>
+        <v>37</v>
       </c>
       <c r="E8" t="n">
-        <v>13.776</v>
+        <v>2.923</v>
       </c>
       <c r="F8" t="n">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="G8" t="n">
-        <v>840000</v>
+        <v>259000</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1496,7 +1621,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
         <v>2</v>
@@ -1507,16 +1632,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="E9" t="n">
-        <v>15.092</v>
+        <v>13.53</v>
       </c>
       <c r="F9" t="n">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="G9" t="n">
-        <v>1078000</v>
+        <v>825000</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1531,56 +1656,56 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Air</t>
+          <t>Ocean</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E10" t="n">
-        <v>15.876</v>
+        <v>15.092</v>
       </c>
       <c r="F10" t="n">
         <v>7000</v>
       </c>
       <c r="G10" t="n">
-        <v>1134000</v>
+        <v>1078000</v>
       </c>
       <c r="H10" t="n">
-        <v>3240</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ocean</t>
+          <t>Air</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="E11" t="n">
-        <v>2.774</v>
+        <v>15.876</v>
       </c>
       <c r="F11" t="n">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="G11" t="n">
-        <v>190000</v>
+        <v>1134000</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="n">
         <v>3</v>
@@ -1591,16 +1716,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E12" t="n">
-        <v>0.225</v>
+        <v>2.774</v>
       </c>
       <c r="F12" t="n">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="G12" t="n">
-        <v>90000</v>
+        <v>190000</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1608,7 +1733,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="n">
         <v>3</v>
@@ -1619,16 +1744,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="E13" t="n">
-        <v>8.6</v>
+        <v>0.225</v>
       </c>
       <c r="F13" t="n">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="G13" t="n">
-        <v>1800000</v>
+        <v>90000</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1636,7 +1761,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
@@ -1647,16 +1772,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>155</v>
+        <v>70</v>
       </c>
       <c r="E14" t="n">
-        <v>9.765000000000001</v>
+        <v>3.01</v>
       </c>
       <c r="F14" t="n">
         <v>9000</v>
       </c>
       <c r="G14" t="n">
-        <v>1395000</v>
+        <v>630000</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1664,7 +1789,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="n">
         <v>3</v>
@@ -1675,16 +1800,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="E15" t="n">
-        <v>2.205</v>
+        <v>9.765000000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="G15" t="n">
-        <v>98000</v>
+        <v>1395000</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1692,7 +1817,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="n">
         <v>3</v>
@@ -1703,16 +1828,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>154</v>
+        <v>49</v>
       </c>
       <c r="E16" t="n">
-        <v>13.244</v>
+        <v>2.205</v>
       </c>
       <c r="F16" t="n">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="G16" t="n">
-        <v>1386000</v>
+        <v>98000</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1720,7 +1845,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
         <v>3</v>
@@ -1731,16 +1856,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="E17" t="n">
-        <v>13.588</v>
+        <v>13.244</v>
       </c>
       <c r="F17" t="n">
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="G17" t="n">
-        <v>1204000</v>
+        <v>1386000</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1748,7 +1873,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="n">
         <v>3</v>
@@ -1759,16 +1884,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="E18" t="n">
-        <v>2.624</v>
+        <v>10.665</v>
       </c>
       <c r="F18" t="n">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="G18" t="n">
-        <v>160000</v>
+        <v>945000</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1776,7 +1901,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="n">
         <v>3</v>
@@ -1787,16 +1912,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="E19" t="n">
-        <v>6.392</v>
+        <v>2.624</v>
       </c>
       <c r="F19" t="n">
-        <v>9000</v>
+        <v>5000</v>
       </c>
       <c r="G19" t="n">
-        <v>846000</v>
+        <v>160000</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1804,29 +1929,57 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>9</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>94</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6.392</v>
+      </c>
+      <c r="F20" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>846000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>10</v>
       </c>
-      <c r="B20" t="n">
-        <v>3</v>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>Ocean</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>199</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E21" t="n">
         <v>19.502</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F21" t="n">
         <v>7000</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G21" t="n">
         <v>1393000</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1885,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>410</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4">
@@ -1907,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>208</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6">
@@ -1929,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>433</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8">
@@ -1940,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>348</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9">
@@ -1962,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>565</v>
+        <v>674</v>
       </c>
     </row>
     <row r="11">
@@ -2006,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15">
@@ -2039,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>356</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18">
@@ -2050,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>212</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19">
@@ -2072,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>489</v>
+        <v>523</v>
       </c>
     </row>
     <row r="21">
@@ -2281,7 +2434,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -2336,7 +2489,7 @@
         <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45">
@@ -2380,7 +2533,7 @@
         <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49">

</xml_diff>

<commit_message>
Refactor heuristic_solution.py to improve holding cost calculations by incorporating costs for arriving shipments. Updated debug output to provide clearer insights into total holding costs and fixed costs for different shipping methods. Adjusted Excel output to reflect these changes.
</commit_message>
<xml_diff>
--- a/heuristic_results.xlsx
+++ b/heuristic_results.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16617176</v>
+        <v>16920316</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1361680</v>
+        <v>1666320</v>
       </c>
     </row>
     <row r="8">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2580</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="9">
@@ -1095,10 +1095,10 @@
         <v>190000</v>
       </c>
       <c r="H2" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I2" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
@@ -1124,10 +1124,10 @@
         <v>90000</v>
       </c>
       <c r="H3" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I3" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
@@ -1153,10 +1153,10 @@
         <v>2538000</v>
       </c>
       <c r="H4" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I4" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
@@ -1182,10 +1182,10 @@
         <v>2268000</v>
       </c>
       <c r="H5" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I5" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -1211,10 +1211,10 @@
         <v>232000</v>
       </c>
       <c r="H6" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I6" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7">
@@ -1240,10 +1240,10 @@
         <v>1386000</v>
       </c>
       <c r="H7" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I7" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8">
@@ -1269,10 +1269,10 @@
         <v>1204000</v>
       </c>
       <c r="H8" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I8" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
@@ -1298,10 +1298,10 @@
         <v>1305000</v>
       </c>
       <c r="H9" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I9" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
@@ -1327,10 +1327,10 @@
         <v>846000</v>
       </c>
       <c r="H10" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I10" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
@@ -1356,10 +1356,10 @@
         <v>5173000</v>
       </c>
       <c r="H11" t="n">
-        <v>136168</v>
+        <v>166632</v>
       </c>
       <c r="I11" t="n">
-        <v>258</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>